<commit_message>
Initial commit of my Streamlit app
</commit_message>
<xml_diff>
--- a/glossary_for_apps.xlsx
+++ b/glossary_for_apps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KEMENKEU\my_streamlit_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B649D08-6C19-4B0D-A6CB-C42480480EF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2512F9C7-5C0C-4AD1-BF7E-E550B0C8FAAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9960" tabRatio="661" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13020" tabRatio="661" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final" sheetId="20" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5024" uniqueCount="2974">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5031" uniqueCount="2981">
   <si>
     <t>SINGKATAN</t>
   </si>
@@ -9904,6 +9904,27 @@
   </si>
   <si>
     <t>Eselon II pada Direktorat Jenderal Perbendaharaan yang mempunyai tugas melaksanakan penyusunan telaahan, kajian, dan rekomendasi di bidang pengelolaan kas, sistem manajemen investasi, dan pembinaan pengelolaan keuangan Badan Layanan Umum.</t>
+  </si>
+  <si>
+    <t>Directorate of Budget Execution</t>
+  </si>
+  <si>
+    <t>Directorate of State Cash Management</t>
+  </si>
+  <si>
+    <t>Directorate of Investment Management System</t>
+  </si>
+  <si>
+    <t>Directorate of Treasury System</t>
+  </si>
+  <si>
+    <t>Directorate of Public Service Agency Financial Management Supervision</t>
+  </si>
+  <si>
+    <t>Directorate of Treasury Information System and Technlogy</t>
+  </si>
+  <si>
+    <t>Advisor to the Director General for Treasury Affairs</t>
   </si>
 </sst>
 </file>
@@ -10742,8 +10763,8 @@
   <dimension ref="A1:F1498"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1362" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1499" sqref="C1499"/>
+      <pane ySplit="1" topLeftCell="A1496" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1498" sqref="F1498"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -32279,6 +32300,9 @@
       <c r="C1492" s="72" t="s">
         <v>2967</v>
       </c>
+      <c r="F1492" t="s">
+        <v>2974</v>
+      </c>
     </row>
     <row r="1493" spans="1:6" ht="43.2">
       <c r="A1493" s="1" t="s">
@@ -32290,6 +32314,9 @@
       <c r="C1493" s="72" t="s">
         <v>2968</v>
       </c>
+      <c r="F1493" t="s">
+        <v>2975</v>
+      </c>
     </row>
     <row r="1494" spans="1:6" ht="43.2">
       <c r="A1494" s="1" t="s">
@@ -32301,6 +32328,9 @@
       <c r="C1494" s="72" t="s">
         <v>2969</v>
       </c>
+      <c r="F1494" t="s">
+        <v>2976</v>
+      </c>
     </row>
     <row r="1495" spans="1:6" ht="43.2">
       <c r="A1495" s="1" t="s">
@@ -32312,6 +32342,9 @@
       <c r="C1495" s="72" t="s">
         <v>2970</v>
       </c>
+      <c r="F1495" t="s">
+        <v>2978</v>
+      </c>
     </row>
     <row r="1496" spans="1:6" ht="43.2">
       <c r="A1496" s="1" t="s">
@@ -32323,6 +32356,9 @@
       <c r="C1496" s="72" t="s">
         <v>2972</v>
       </c>
+      <c r="F1496" t="s">
+        <v>2977</v>
+      </c>
     </row>
     <row r="1497" spans="1:6" ht="43.2">
       <c r="A1497" s="1" t="s">
@@ -32334,6 +32370,9 @@
       <c r="C1497" s="72" t="s">
         <v>2971</v>
       </c>
+      <c r="F1497" t="s">
+        <v>2979</v>
+      </c>
     </row>
     <row r="1498" spans="1:6" ht="57.6">
       <c r="A1498" s="1" t="s">
@@ -32344,6 +32383,9 @@
       </c>
       <c r="C1498" s="72" t="s">
         <v>2973</v>
+      </c>
+      <c r="F1498" t="s">
+        <v>2980</v>
       </c>
     </row>
   </sheetData>
@@ -32360,6 +32402,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="b2992bec-f44b-42ac-b395-58539b0a572b" xsi:nil="true"/>
@@ -32368,15 +32419,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -32615,20 +32657,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3875F7EC-542E-4005-A09B-C0B7A5DBBE35}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C336D443-AFDD-4577-90DC-A3FE0CF59561}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="b2992bec-f44b-42ac-b395-58539b0a572b"/>
     <ds:schemaRef ds:uri="0292f133-7a09-4a66-b08d-3ae74d4bae5f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3875F7EC-542E-4005-A09B-C0B7A5DBBE35}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>